<commit_message>
copied movies to supplement directory
</commit_message>
<xml_diff>
--- a/supplement/Supplementary_Table_2.xlsx
+++ b/supplement/Supplementary_Table_2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwd7/repos/siph_skimming/supplement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{568B0E43-023E-EC46-863E-8B77FE45FD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E3FF0F-6293-C84C-84B9-8666A7A76289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1100" windowWidth="27240" windowHeight="16140"/>
+    <workbookView xWindow="1000" yWindow="1100" windowWidth="27240" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplementary_Table_2" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="78">
   <si>
     <t>sample</t>
   </si>
@@ -272,9 +272,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -762,7 +762,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1119,11 +1119,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1261,11 +1261,11 @@
         <v>1.0432119237666666</v>
       </c>
       <c r="D2" s="4">
-        <f>Y2/1000000</f>
+        <f t="shared" ref="D2:D36" si="0">Y2/1000000</f>
         <v>106.342097</v>
       </c>
       <c r="E2" s="3">
-        <f>Z2/1000000000</f>
+        <f t="shared" ref="E2:E36" si="1">Z2/1000000000</f>
         <v>31.296357712999999</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1371,11 +1371,11 @@
         <v>1.0221936803333334</v>
       </c>
       <c r="D3" s="4">
-        <f>Y3/1000000</f>
+        <f t="shared" si="0"/>
         <v>103.93870200000001</v>
       </c>
       <c r="E3" s="3">
-        <f>Z3/1000000000</f>
+        <f t="shared" si="1"/>
         <v>30.665810409999999</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1481,11 +1481,11 @@
         <v>0.95887309086666672</v>
       </c>
       <c r="D4" s="4">
-        <f>Y4/1000000</f>
+        <f t="shared" si="0"/>
         <v>96.986594999999994</v>
       </c>
       <c r="E4" s="3">
-        <f>Z4/1000000000</f>
+        <f t="shared" si="1"/>
         <v>28.766192726</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -1591,11 +1591,11 @@
         <v>76</v>
       </c>
       <c r="D5" s="4">
-        <f>Y5/1000000</f>
+        <f t="shared" si="0"/>
         <v>1034.742285</v>
       </c>
       <c r="E5" s="3">
-        <f>Z5/1000000000</f>
+        <f t="shared" si="1"/>
         <v>308</v>
       </c>
       <c r="F5" s="3">
@@ -1702,11 +1702,11 @@
         <v>76</v>
       </c>
       <c r="D6" s="4">
-        <f>Y6/1000000</f>
+        <f t="shared" si="0"/>
         <v>255.281758</v>
       </c>
       <c r="E6" s="3">
-        <f>Z6/1000000000</f>
+        <f t="shared" si="1"/>
         <v>72.973417105999999</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1812,11 +1812,11 @@
         <v>2.2343956695</v>
       </c>
       <c r="D7" s="4">
-        <f>Y7/1000000</f>
+        <f t="shared" si="0"/>
         <v>249.82133899999999</v>
       </c>
       <c r="E7" s="3">
-        <f>Z7/1000000000</f>
+        <f t="shared" si="1"/>
         <v>67.031870084999994</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1922,11 +1922,11 @@
         <v>1.3388302877</v>
       </c>
       <c r="D8" s="4">
-        <f>Y8/1000000</f>
+        <f t="shared" si="0"/>
         <v>145.57233199999999</v>
       </c>
       <c r="E8" s="3">
-        <f>Z8/1000000000</f>
+        <f t="shared" si="1"/>
         <v>40.164908631000003</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -2032,11 +2032,11 @@
         <v>2.8869055793333334</v>
       </c>
       <c r="D9" s="4">
-        <f>Y9/1000000</f>
+        <f t="shared" si="0"/>
         <v>299.47044199999999</v>
       </c>
       <c r="E9" s="3">
-        <f>Z9/1000000000</f>
+        <f t="shared" si="1"/>
         <v>86.607167380000007</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -2142,11 +2142,11 @@
         <v>1.4163818856333334</v>
       </c>
       <c r="D10" s="4">
-        <f>Y10/1000000</f>
+        <f t="shared" si="0"/>
         <v>150.626304</v>
       </c>
       <c r="E10" s="3">
-        <f>Z10/1000000000</f>
+        <f t="shared" si="1"/>
         <v>42.491456569</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -2252,11 +2252,11 @@
         <v>76</v>
       </c>
       <c r="D11" s="4">
-        <f>Y11/1000000</f>
+        <f t="shared" si="0"/>
         <v>353.18907999999999</v>
       </c>
       <c r="E11" s="3">
-        <f>Z11/1000000000</f>
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
       <c r="F11" s="3">
@@ -2364,11 +2364,11 @@
         <v>2.0758092502999999</v>
       </c>
       <c r="D12" s="4">
-        <f>Y12/1000000</f>
+        <f t="shared" si="0"/>
         <v>221.27956499999999</v>
       </c>
       <c r="E12" s="3">
-        <f>Z12/1000000000</f>
+        <f t="shared" si="1"/>
         <v>62.274277509000001</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -2474,11 +2474,11 @@
         <v>76</v>
       </c>
       <c r="D13" s="4">
-        <f>Y13/1000000</f>
+        <f t="shared" si="0"/>
         <v>150.79417699999999</v>
       </c>
       <c r="E13" s="3">
-        <f>Z13/1000000000</f>
+        <f t="shared" si="1"/>
         <v>43.829975720999997</v>
       </c>
       <c r="F13" s="3">
@@ -2586,11 +2586,11 @@
         <v>1.6331117712000001</v>
       </c>
       <c r="D14" s="4">
-        <f>Y14/1000000</f>
+        <f t="shared" si="0"/>
         <v>170.722058</v>
       </c>
       <c r="E14" s="3">
-        <f>Z14/1000000000</f>
+        <f t="shared" si="1"/>
         <v>48.993353136000003</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -2696,11 +2696,11 @@
         <v>1.9326008648666666</v>
       </c>
       <c r="D15" s="4">
-        <f>Y15/1000000</f>
+        <f t="shared" si="0"/>
         <v>198.25357500000001</v>
       </c>
       <c r="E15" s="3">
-        <f>Z15/1000000000</f>
+        <f t="shared" si="1"/>
         <v>57.978025946000002</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -2806,11 +2806,11 @@
         <v>3.0667127445000002</v>
       </c>
       <c r="D16" s="4">
-        <f>Y16/1000000</f>
+        <f t="shared" si="0"/>
         <v>331.33226999999999</v>
       </c>
       <c r="E16" s="3">
-        <f>Z16/1000000000</f>
+        <f t="shared" si="1"/>
         <v>92.001382335000002</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -2916,11 +2916,11 @@
         <v>2.4744798354999999</v>
       </c>
       <c r="D17" s="4">
-        <f>Y17/1000000</f>
+        <f t="shared" si="0"/>
         <v>267.534289</v>
       </c>
       <c r="E17" s="3">
-        <f>Z17/1000000000</f>
+        <f t="shared" si="1"/>
         <v>74.234395065000001</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -3026,11 +3026,11 @@
         <v>2.5719904415333334</v>
       </c>
       <c r="D18" s="4">
-        <f>Y18/1000000</f>
+        <f t="shared" si="0"/>
         <v>284.04904399999998</v>
       </c>
       <c r="E18" s="3">
-        <f>Z18/1000000000</f>
+        <f t="shared" si="1"/>
         <v>77.159713245999995</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -3128,19 +3128,18 @@
       <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="3">
-        <f>AVERAGE(M19:N19)/1000000000</f>
-        <v>2.3338563195000002</v>
+      <c r="B19" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D19" s="4">
-        <f>Y19/1000000</f>
+        <f t="shared" si="0"/>
         <v>878.094696</v>
       </c>
       <c r="E19" s="3">
-        <f>Z19/1000000000</f>
+        <f t="shared" si="1"/>
         <v>256</v>
       </c>
       <c r="F19" s="3">
@@ -3248,11 +3247,11 @@
         <v>1.6680351888</v>
       </c>
       <c r="D20" s="4">
-        <f>Y20/1000000</f>
+        <f t="shared" si="0"/>
         <v>170.90492699999999</v>
       </c>
       <c r="E20" s="3">
-        <f>Z20/1000000000</f>
+        <f t="shared" si="1"/>
         <v>50.041055663999998</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -3358,11 +3357,11 @@
         <v>1.0256975171333333</v>
       </c>
       <c r="D21" s="4">
-        <f>Y21/1000000</f>
+        <f t="shared" si="0"/>
         <v>103.78552500000001</v>
       </c>
       <c r="E21" s="3">
-        <f>Z21/1000000000</f>
+        <f t="shared" si="1"/>
         <v>30.770925514000002</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -3468,11 +3467,11 @@
         <v>2.4361880179000002</v>
       </c>
       <c r="D22" s="4">
-        <f>Y22/1000000</f>
+        <f t="shared" si="0"/>
         <v>266.03637700000002</v>
       </c>
       <c r="E22" s="3">
-        <f>Z22/1000000000</f>
+        <f t="shared" si="1"/>
         <v>73.085640537000003</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -3578,11 +3577,11 @@
         <v>2.6808606277333329</v>
       </c>
       <c r="D23" s="4">
-        <f>Y23/1000000</f>
+        <f t="shared" si="0"/>
         <v>282.74325099999999</v>
       </c>
       <c r="E23" s="3">
-        <f>Z23/1000000000</f>
+        <f t="shared" si="1"/>
         <v>80.425818832000004</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -3688,11 +3687,11 @@
         <v>76</v>
       </c>
       <c r="D24" s="4">
-        <f>Y24/1000000</f>
+        <f t="shared" si="0"/>
         <v>312.83166699999998</v>
       </c>
       <c r="E24" s="3">
-        <f>Z24/1000000000</f>
+        <f t="shared" si="1"/>
         <v>92.498995049000001</v>
       </c>
       <c r="F24" s="3">
@@ -3800,11 +3799,11 @@
         <v>76</v>
       </c>
       <c r="D25" s="4">
-        <f>Y25/1000000</f>
+        <f t="shared" si="0"/>
         <v>290.02642200000003</v>
       </c>
       <c r="E25" s="3">
-        <f>Z25/1000000000</f>
+        <f t="shared" si="1"/>
         <v>86.474099796000004</v>
       </c>
       <c r="F25" s="3">
@@ -3912,11 +3911,11 @@
         <v>76</v>
       </c>
       <c r="D26" s="4">
-        <f>Y26/1000000</f>
+        <f t="shared" si="0"/>
         <v>663.88213499999995</v>
       </c>
       <c r="E26" s="3">
-        <f>Z26/1000000000</f>
+        <f t="shared" si="1"/>
         <v>185</v>
       </c>
       <c r="F26" s="3">
@@ -4024,11 +4023,11 @@
         <v>2.1991171323333334</v>
       </c>
       <c r="D27" s="4">
-        <f>Y27/1000000</f>
+        <f t="shared" si="0"/>
         <v>229.18460899999999</v>
       </c>
       <c r="E27" s="3">
-        <f>Z27/1000000000</f>
+        <f t="shared" si="1"/>
         <v>65.973513969999999</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -4134,11 +4133,11 @@
         <v>2.2287114900666665</v>
       </c>
       <c r="D28" s="4">
-        <f>Y28/1000000</f>
+        <f t="shared" si="0"/>
         <v>235.93160599999999</v>
       </c>
       <c r="E28" s="3">
-        <f>Z28/1000000000</f>
+        <f t="shared" si="1"/>
         <v>66.861344701999997</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -4244,11 +4243,11 @@
         <v>3.7</v>
       </c>
       <c r="D29" s="4">
-        <f>Y29/1000000</f>
+        <f t="shared" si="0"/>
         <v>383.25560200000001</v>
       </c>
       <c r="E29" s="3">
-        <f>Z29/1000000000</f>
+        <f t="shared" si="1"/>
         <v>111</v>
       </c>
       <c r="F29" s="3" t="s">
@@ -4353,11 +4352,11 @@
         <v>76</v>
       </c>
       <c r="D30" s="4">
-        <f>Y30/1000000</f>
+        <f t="shared" si="0"/>
         <v>167.27775</v>
       </c>
       <c r="E30" s="3">
-        <f>Z30/1000000000</f>
+        <f t="shared" si="1"/>
         <v>46.814267661000002</v>
       </c>
       <c r="F30" s="3" t="s">
@@ -4463,11 +4462,11 @@
         <v>76</v>
       </c>
       <c r="D31" s="4">
-        <f>Y31/1000000</f>
+        <f t="shared" si="0"/>
         <v>566.16018599999995</v>
       </c>
       <c r="E31" s="3">
-        <f>Z31/1000000000</f>
+        <f t="shared" si="1"/>
         <v>157</v>
       </c>
       <c r="F31" s="3">
@@ -4575,11 +4574,11 @@
         <v>2.2949540375999997</v>
       </c>
       <c r="D32" s="4">
-        <f>Y32/1000000</f>
+        <f t="shared" si="0"/>
         <v>238.482293</v>
       </c>
       <c r="E32" s="3">
-        <f>Z32/1000000000</f>
+        <f t="shared" si="1"/>
         <v>68.848621128000005</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -4685,11 +4684,11 @@
         <v>1.5764916582333333</v>
       </c>
       <c r="D33" s="4">
-        <f>Y33/1000000</f>
+        <f t="shared" si="0"/>
         <v>159.073318</v>
       </c>
       <c r="E33" s="3">
-        <f>Z33/1000000000</f>
+        <f t="shared" si="1"/>
         <v>47.294749746999997</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -4795,11 +4794,11 @@
         <v>0.99351940116666659</v>
       </c>
       <c r="D34" s="4">
-        <f>Y34/1000000</f>
+        <f t="shared" si="0"/>
         <v>101.191857</v>
       </c>
       <c r="E34" s="3">
-        <f>Z34/1000000000</f>
+        <f t="shared" si="1"/>
         <v>29.805582035</v>
       </c>
       <c r="F34" s="3" t="s">
@@ -4905,11 +4904,11 @@
         <v>2.0915138305999998</v>
       </c>
       <c r="D35" s="4">
-        <f>Y35/1000000</f>
+        <f t="shared" si="0"/>
         <v>219.048236</v>
       </c>
       <c r="E35" s="3">
-        <f>Z35/1000000000</f>
+        <f t="shared" si="1"/>
         <v>62.745414918000002</v>
       </c>
       <c r="F35" s="3" t="s">
@@ -5015,11 +5014,11 @@
         <v>1.6031074187666667</v>
       </c>
       <c r="D36" s="4">
-        <f>Y36/1000000</f>
+        <f t="shared" si="0"/>
         <v>169.177559</v>
       </c>
       <c r="E36" s="3">
-        <f>Z36/1000000000</f>
+        <f t="shared" si="1"/>
         <v>48.093222562999998</v>
       </c>
       <c r="F36" s="3" t="s">

</xml_diff>

<commit_message>
updated minimum genome size estimates
</commit_message>
<xml_diff>
--- a/supplement/Supplementary_Table_2.xlsx
+++ b/supplement/Supplementary_Table_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwd7/repos/siph_skimming/supplement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwd7\repos\siph_skimming\supplement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1A13F6-3FBE-FE4E-912F-83DD3E0069DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62E7B5E-F885-463B-92AD-D8A6B5E08BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1100" windowWidth="27240" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20505" yWindow="120" windowWidth="26558" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplementary_Table_2" sheetId="1" r:id="rId1"/>
@@ -1122,27 +1122,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" customWidth="1"/>
-    <col min="25" max="25" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.375" customWidth="1"/>
+    <col min="3" max="3" width="31.625" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="6" max="6" width="16.875" customWidth="1"/>
+    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.625" customWidth="1"/>
+    <col min="14" max="14" width="15.125" customWidth="1"/>
+    <col min="25" max="25" width="18.125" customWidth="1"/>
     <col min="26" max="26" width="20" customWidth="1"/>
     <col min="34" max="34" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1257,8 +1257,8 @@
         <v>75</v>
       </c>
       <c r="C2" s="3">
-        <f>Z2/30/1000000000</f>
-        <v>1.0432119237666666</v>
+        <f>Z2/20/1000000000</f>
+        <v>1.5648178856500001</v>
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2:D36" si="0">Y2/1000000</f>
@@ -1359,7 +1359,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1367,8 +1367,8 @@
         <v>75</v>
       </c>
       <c r="C3" s="3">
-        <f>Z3/30/1000000000</f>
-        <v>1.0221936803333334</v>
+        <f t="shared" ref="C3:C4" si="2">Z3/20/1000000000</f>
+        <v>1.5332905205</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" si="0"/>
@@ -1469,7 +1469,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1477,8 +1477,8 @@
         <v>75</v>
       </c>
       <c r="C4" s="3">
-        <f>Z4/30/1000000000</f>
-        <v>0.95887309086666672</v>
+        <f t="shared" si="2"/>
+        <v>1.4383096362999999</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="0"/>
@@ -1579,7 +1579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1808,8 +1808,8 @@
         <v>75</v>
       </c>
       <c r="C7" s="3">
-        <f>Z7/30/1000000000</f>
-        <v>2.2343956695</v>
+        <f t="shared" ref="C7:C23" si="3">Z7/20/1000000000</f>
+        <v>3.3515935042499998</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
@@ -1910,7 +1910,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1918,8 +1918,8 @@
         <v>75</v>
       </c>
       <c r="C8" s="3">
-        <f>Z8/30/1000000000</f>
-        <v>1.3388302877</v>
+        <f t="shared" si="3"/>
+        <v>2.0082454315499998</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
@@ -2020,7 +2020,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -2028,8 +2028,8 @@
         <v>75</v>
       </c>
       <c r="C9" s="3">
-        <f>Z9/30/1000000000</f>
-        <v>2.8869055793333334</v>
+        <f t="shared" si="3"/>
+        <v>4.3303583689999998</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
@@ -2130,7 +2130,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2138,8 +2138,8 @@
         <v>75</v>
       </c>
       <c r="C10" s="3">
-        <f>Z10/30/1000000000</f>
-        <v>1.4163818856333334</v>
+        <f t="shared" si="3"/>
+        <v>2.1245728284499998</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
@@ -2240,7 +2240,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2360,8 +2360,8 @@
         <v>75</v>
       </c>
       <c r="C12" s="3">
-        <f>Z12/30/1000000000</f>
-        <v>2.0758092502999999</v>
+        <f t="shared" si="3"/>
+        <v>3.1137138754499998</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="0"/>
@@ -2462,7 +2462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2582,8 +2582,8 @@
         <v>75</v>
       </c>
       <c r="C14" s="3">
-        <f>Z14/30/1000000000</f>
-        <v>1.6331117712000001</v>
+        <f t="shared" si="3"/>
+        <v>2.4496676568</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="0"/>
@@ -2684,7 +2684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2692,8 +2692,8 @@
         <v>75</v>
       </c>
       <c r="C15" s="3">
-        <f>Z15/30/1000000000</f>
-        <v>1.9326008648666666</v>
+        <f t="shared" si="3"/>
+        <v>2.8989012973000001</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="0"/>
@@ -2794,7 +2794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2802,8 +2802,8 @@
         <v>75</v>
       </c>
       <c r="C16" s="3">
-        <f>Z16/30/1000000000</f>
-        <v>3.0667127445000002</v>
+        <f t="shared" si="3"/>
+        <v>4.6000691167500003</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="0"/>
@@ -2904,7 +2904,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2912,8 +2912,8 @@
         <v>75</v>
       </c>
       <c r="C17" s="3">
-        <f>Z17/30/1000000000</f>
-        <v>2.4744798354999999</v>
+        <f t="shared" si="3"/>
+        <v>3.7117197532500001</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="0"/>
@@ -3014,7 +3014,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -3022,8 +3022,8 @@
         <v>75</v>
       </c>
       <c r="C18" s="3">
-        <f>Z18/30/1000000000</f>
-        <v>2.5719904415333334</v>
+        <f t="shared" si="3"/>
+        <v>3.8579856623000004</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="0"/>
@@ -3124,7 +3124,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -3244,8 +3244,8 @@
         <v>75</v>
       </c>
       <c r="C20" s="3">
-        <f>Z20/30/1000000000</f>
-        <v>1.6680351888</v>
+        <f t="shared" si="3"/>
+        <v>2.5020527831999999</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="0"/>
@@ -3346,7 +3346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -3354,8 +3354,8 @@
         <v>75</v>
       </c>
       <c r="C21" s="3">
-        <f>Z21/30/1000000000</f>
-        <v>1.0256975171333333</v>
+        <f t="shared" si="3"/>
+        <v>1.5385462757000001</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="0"/>
@@ -3456,7 +3456,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -3464,8 +3464,8 @@
         <v>75</v>
       </c>
       <c r="C22" s="3">
-        <f>Z22/30/1000000000</f>
-        <v>2.4361880179000002</v>
+        <f>Z22/20/1000000000</f>
+        <v>3.6542820268499998</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="0"/>
@@ -3566,7 +3566,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -3574,8 +3574,8 @@
         <v>75</v>
       </c>
       <c r="C23" s="3">
-        <f>Z23/30/1000000000</f>
-        <v>2.6808606277333329</v>
+        <f>Z23/20/1000000000</f>
+        <v>4.0212909416000002</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="0"/>
@@ -3676,7 +3676,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -4020,8 +4020,8 @@
         <v>75</v>
       </c>
       <c r="C27" s="3">
-        <f>Z27/30/1000000000</f>
-        <v>2.1991171323333334</v>
+        <f>Z27/20/1000000000</f>
+        <v>3.2986756984999999</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="0"/>
@@ -4122,7 +4122,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -4130,8 +4130,8 @@
         <v>75</v>
       </c>
       <c r="C28" s="3">
-        <f>Z28/30/1000000000</f>
-        <v>2.2287114900666665</v>
+        <f t="shared" ref="C28:C29" si="4">Z28/20/1000000000</f>
+        <v>3.3430672350999999</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="0"/>
@@ -4232,7 +4232,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -4240,8 +4240,8 @@
         <v>75</v>
       </c>
       <c r="C29" s="3">
-        <f>Z29/30/1000000000</f>
-        <v>3.7</v>
+        <f t="shared" si="4"/>
+        <v>5.55</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="0"/>
@@ -4342,7 +4342,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -4571,8 +4571,8 @@
         <v>75</v>
       </c>
       <c r="C32" s="3">
-        <f>Z32/30/1000000000</f>
-        <v>2.2949540375999997</v>
+        <f t="shared" ref="C32:C36" si="5">Z32/20/1000000000</f>
+        <v>3.4424310564000002</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="0"/>
@@ -4673,7 +4673,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -4681,8 +4681,8 @@
         <v>75</v>
       </c>
       <c r="C33" s="3">
-        <f>Z33/30/1000000000</f>
-        <v>1.5764916582333333</v>
+        <f t="shared" si="5"/>
+        <v>2.3647374873499998</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="0"/>
@@ -4783,7 +4783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -4791,8 +4791,8 @@
         <v>75</v>
       </c>
       <c r="C34" s="3">
-        <f>Z34/30/1000000000</f>
-        <v>0.99351940116666659</v>
+        <f t="shared" si="5"/>
+        <v>1.4902791017499999</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="0"/>
@@ -4893,7 +4893,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -4901,8 +4901,8 @@
         <v>75</v>
       </c>
       <c r="C35" s="3">
-        <f>Z35/30/1000000000</f>
-        <v>2.0915138305999998</v>
+        <f t="shared" si="5"/>
+        <v>3.1372707459</v>
       </c>
       <c r="D35" s="4">
         <f t="shared" si="0"/>
@@ -5003,7 +5003,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -5011,8 +5011,8 @@
         <v>75</v>
       </c>
       <c r="C36" s="3">
-        <f>Z36/30/1000000000</f>
-        <v>1.6031074187666667</v>
+        <f t="shared" si="5"/>
+        <v>2.4046611281499999</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="0"/>

</xml_diff>